<commit_message>
update code for new tournaments as of 3/20/24
</commit_message>
<xml_diff>
--- a/OlympicRankings.xlsx
+++ b/OlympicRankings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmspr\Documents\Me\Projects\olympic-beach-volleyball-rankings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2627E4-4CC5-406D-827B-26B9B56824A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF16F054-F9FB-48AE-B4E0-B27BEFD22A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{B079F3EF-72BC-FD4B-A18A-1DECC4C0091B}"/>
   </bookViews>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3AB935-CC39-D24D-B8C8-63A01B751BCD}">
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="112" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1346,7 +1346,7 @@
         <v>163</v>
       </c>
       <c r="C2" s="5">
-        <f t="shared" ref="C2:C33" si="0">SUM(D2:AB2)</f>
+        <f t="shared" ref="C2:D33" si="0">SUM(D2:AB2)</f>
         <v>9460</v>
       </c>
       <c r="K2">
@@ -5023,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F3D6D1-4228-FD4A-83DE-0D9F79CF7314}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>